<commit_message>
a pcb is born
</commit_message>
<xml_diff>
--- a/POC DAC/CalculsFreq.xlsx
+++ b/POC DAC/CalculsFreq.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocal\Desktop\Elec_Synthe\POC DAC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="320" yWindow="2280" windowWidth="14380" windowHeight="12780" tabRatio="500"/>
+    <workbookView xWindow="315" yWindow="2280" windowWidth="14385" windowHeight="12780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>15-24</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -82,9 +90,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -97,6 +106,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -422,23 +439,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I27"/>
+  <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8000000</v>
       </c>
@@ -452,7 +471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>6144000</v>
       </c>
@@ -461,7 +480,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>1/B5</f>
         <v>1.6276041666666666E-7</v>
@@ -470,8 +489,14 @@
         <f t="shared" ref="D6" si="0">1/D5</f>
         <v>1.5624999999999999E-8</v>
       </c>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>B6/2</f>
         <v>8.1380208333333331E-8</v>
@@ -484,8 +509,32 @@
         <f>32*48000</f>
         <v>1536000</v>
       </c>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="I7">
+        <v>12288000</v>
+      </c>
+      <c r="J7">
+        <f>I7/J6</f>
+        <v>4096000</v>
+      </c>
+      <c r="K7">
+        <f>J7*K6</f>
+        <v>73728000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f>1/I7</f>
+        <v>8.1380208333333331E-8</v>
+      </c>
+      <c r="K8">
+        <f>1/K7</f>
+        <v>1.3563368055555556E-8</v>
+      </c>
+      <c r="M8">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <f>(D5/(2*F7)) - 1</f>
         <v>19.833333333333332</v>
@@ -502,8 +551,18 @@
         <f>F9/32</f>
         <v>50000</v>
       </c>
-    </row>
-    <row r="10" spans="2:9">
+      <c r="K9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>48000</v>
+      </c>
+      <c r="M9">
+        <f>L9*M8</f>
+        <v>9216000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F10">
         <f>F9-F7</f>
         <v>64000</v>
@@ -512,25 +571,33 @@
         <f>G9*128</f>
         <v>6400000</v>
       </c>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="M10">
+        <f>1/M9</f>
+        <v>1.0850694444444445E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F11">
         <f>(F10/F9)*100</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="M11">
+        <f>M10/K8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C12">
         <f>(D5/(2*G10)) - 1</f>
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>80000000</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>1/B14</f>
         <v>1.2499999999999999E-8</v>
@@ -540,13 +607,13 @@
         <v>654.87884741322853</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f>12*B15</f>
         <v>1.4999999999999999E-7</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>1/B16</f>
         <v>6666666.666666667</v>
@@ -564,7 +631,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>C17*32</f>
         <v>1666666.6666666667</v>
@@ -574,7 +641,7 @@
         <v>833333.33333333337</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C19">
         <f>B14/C18</f>
         <v>48</v>
@@ -592,7 +659,7 @@
         <v>1.9199999999999999E-5</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F20">
         <f>F19/B15</f>
         <v>96</v>
@@ -602,7 +669,7 @@
         <v>9.5999999999999996E-6</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <f>1/C18</f>
         <v>5.9999999999999997E-7</v>
@@ -612,7 +679,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <f>C21*16</f>
         <v>9.5999999999999996E-6</v>
@@ -622,19 +689,19 @@
         <v>2.2883295194508011</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G25">
         <f>24*2</f>
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G26">
         <f>B14/48</f>
         <v>1666666.6666666667</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G27">
         <f>1/G26</f>
         <v>5.9999999999999997E-7</v>

</xml_diff>